<commit_message>
1. Updating query syntax to OR and AND (keeping / for synonims) 2. Fixing autosave issues
</commit_message>
<xml_diff>
--- a/episomer/inst/extdata/topics.xlsx
+++ b/episomer/inst/extdata/topics.xlsx
@@ -52,14 +52,13 @@
     <t xml:space="preserve">Measles</t>
   </si>
   <si>
-    <t xml:space="preserve">measles/sarampion/rougeole/sarampo/gafeira/morrinha,
--fake</t>
+    <t xml:space="preserve">measles OR sarampion OR rougeole OR sarampo OR gafeira OR morrinha</t>
   </si>
   <si>
     <t xml:space="preserve">COVID-19</t>
   </si>
   <si>
-    <t xml:space="preserve">coronavirus/"novel coronavirus"/ncov/"2019-ncov"/covid-19/sars-covid-2/"nuevo coronavirus"/"nouveau coronavirus"/"novo coronavirus"</t>
+    <t xml:space="preserve">coronavirus OR "novel coronavirus" OR ncov OR "2019-ncov" OR covid-19 OR sars-covid-2 OR "nuevo coronavirus" OR "nouveau coronavirus" OR "novo coronavirus"</t>
   </si>
   <si>
     <t xml:space="preserve">COVID-19 outbreaks</t>
@@ -73,8 +72,35 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">coronavirus/"novel coronavirus"/covid-19/sars-covid-2/covid19, 
-outbreak/cluster/school/hospital/university/variant)
+      <t xml:space="preserve">coronavirus AND </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">outbreak/cluster/school</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> OR covid-19 AND </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">outbreak/cluster/school
 </t>
     </r>
     <r>
@@ -83,6 +109,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-fake</t>
     </r>
@@ -350,10 +377,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -420,11 +447,11 @@
       </c>
       <c r="G2" s="4" t="n">
         <f aca="false">LEN(F2)</f>
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="H2" s="4" t="n">
         <f aca="false">LEN(TRIM(F2))-LEN(SUBSTITUTE(F2," ",""))+1</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1</v>
@@ -451,7 +478,7 @@
       </c>
       <c r="G3" s="4" t="n">
         <f aca="false">LEN(F3)</f>
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -476,7 +503,7 @@
       </c>
       <c r="G4" s="4" t="n">
         <f aca="false">LEN(F4)</f>
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="H4" s="4"/>
     </row>

</xml_diff>